<commit_message>
Task7. 8.Deleted all stored procedures from SQLServer.Database.
</commit_message>
<xml_diff>
--- a/Task7/xlsTable/Task7.xlsx
+++ b/Task7/xlsTable/Task7.xlsx
@@ -1586,8 +1586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1602,6 +1602,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1">
+        <v>6</v>
+      </c>
       <c r="J1">
         <v>1</v>
       </c>
@@ -1789,6 +1792,12 @@
       <c r="C7">
         <v>3</v>
       </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="L7">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C8" s="54" t="s">
@@ -1926,7 +1935,11 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>7</v>
+      </c>
+    </row>
     <row r="14" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="54" t="s">
         <v>25</v>

</xml_diff>